<commit_message>
Updating database with favourites and ratings
</commit_message>
<xml_diff>
--- a/database/data/recipe-tables.xlsx
+++ b/database/data/recipe-tables.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ASettle/University/recipe-database/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ASettle/University/recipe-database/database/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E7C435-EF51-7E46-860C-2DD0815711D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1E64A9-B5D7-884B-A24B-AF0103A9D6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" activeTab="4" xr2:uid="{2C3B1045-9B82-AB42-894A-40C0C009013B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" activeTab="5" xr2:uid="{2C3B1045-9B82-AB42-894A-40C0C009013B}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="12" r:id="rId1"/>
-    <sheet name="roles" sheetId="13" r:id="rId2"/>
-    <sheet name="recipe" sheetId="1" r:id="rId3"/>
-    <sheet name="cooking_time" sheetId="11" r:id="rId4"/>
-    <sheet name="rating" sheetId="10" r:id="rId5"/>
-    <sheet name="steps" sheetId="9" r:id="rId6"/>
-    <sheet name="category" sheetId="2" r:id="rId7"/>
-    <sheet name="course" sheetId="3" r:id="rId8"/>
-    <sheet name="ingredients" sheetId="7" r:id="rId9"/>
-    <sheet name="quantity" sheetId="8" r:id="rId10"/>
+    <sheet name="favourite" sheetId="14" r:id="rId2"/>
+    <sheet name="roles" sheetId="13" r:id="rId3"/>
+    <sheet name="recipe" sheetId="1" r:id="rId4"/>
+    <sheet name="cooking_time" sheetId="11" r:id="rId5"/>
+    <sheet name="rating" sheetId="10" r:id="rId6"/>
+    <sheet name="steps" sheetId="9" r:id="rId7"/>
+    <sheet name="category" sheetId="2" r:id="rId8"/>
+    <sheet name="course" sheetId="3" r:id="rId9"/>
+    <sheet name="ingredients" sheetId="7" r:id="rId10"/>
+    <sheet name="quantity" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="213">
   <si>
     <t>recipe_id</t>
   </si>
@@ -681,6 +682,9 @@
   </si>
   <si>
     <t>$2y$15$Fwz88Z/0TX3j14vyI2CJFekMglhZhM8/mAH7MddvqJtJ5HSRRPCNi</t>
+  </si>
+  <si>
+    <t>favourite_id</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1115,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1392,6 +1396,663 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4C9008-147A-1C47-A047-994632265275}">
+  <dimension ref="A1:E58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="15">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="15">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="15">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="15">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="15">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="15">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="15">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="15">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="15">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="15">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="15">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="15">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="15">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="15">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="15">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="15">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="15">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="15">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="15">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="15">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="15">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="15">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="15">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="15">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="15">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D4854F-98D8-954C-A3D6-8F575E3228E3}">
   <dimension ref="A1:E69"/>
   <sheetViews>
@@ -2561,6 +3222,296 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FFA78F-0293-AF48-ACE7-3E054D4A5F26}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>7</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAA86F1-3111-0C42-8A6C-6E3FBB30916D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2599,12 +3550,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C0D58F-BCD3-684D-A12D-6D0C5DE84C56}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2785,7 +3736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B238CB-A307-0B45-B59E-6C29AFD6AD5D}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2964,84 +3915,377 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0237C7E1-52F7-E745-931F-FF3F1E85620A}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4.5</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>4.5</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C5">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C6">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
         <v>4.5</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4.5</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3.5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3049,11 +4293,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADAC809-9D70-E946-80A3-A7B384091D4F}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3447,7 +4691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7BCA32-7096-884F-89B9-A6D8B5672DF7}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -3570,7 +4814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FD7EFF-DEF3-6E44-B041-B4F79B5146F8}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -3706,661 +4950,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4C9008-147A-1C47-A047-994632265275}">
-  <dimension ref="A1:E58"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>2</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15">
-        <v>4</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
-        <v>5</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
-        <v>6</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
-        <v>8</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
-        <v>9</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
-        <v>10</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <v>11</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15">
-        <v>12</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
-        <v>13</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="15">
-        <v>16</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
-        <v>17</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="15">
-        <v>18</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="15">
-        <v>19</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="15">
-        <v>20</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="15">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="15">
-        <v>22</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="15">
-        <v>23</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="15">
-        <v>24</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="15">
-        <v>25</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="15">
-        <v>26</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="15">
-        <v>27</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="15">
-        <v>28</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="15">
-        <v>29</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="15">
-        <v>30</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="15">
-        <v>31</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="15">
-        <v>32</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="15">
-        <v>33</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="15">
-        <v>34</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="15">
-        <v>35</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="15">
-        <v>36</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="15">
-        <v>37</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="15">
-        <v>38</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="15">
-        <v>39</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="15">
-        <v>40</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="15">
-        <v>41</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="15">
-        <v>42</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="15">
-        <v>43</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="15">
-        <v>44</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="15">
-        <v>45</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="15">
-        <v>46</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="15">
-        <v>47</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="15">
-        <v>48</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="15">
-        <v>49</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="15">
-        <v>50</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="15">
-        <v>51</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="15">
-        <v>52</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="15">
-        <v>53</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="15">
-        <v>54</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="15">
-        <v>55</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="15">
-        <v>56</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="15">
-        <v>57</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>